<commit_message>
update to ACA inclusion and addition of PCAs in MNI space
</commit_message>
<xml_diff>
--- a/colormaps/dkt_areas.xlsx
+++ b/colormaps/dkt_areas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m206305/Documents/data/BrainBeat/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m206305/Documents/git/BrainBeat/colormaps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FEC9AC5-36DC-8643-8DB2-C1D8F4D5A6C7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA5856AE-1116-FB45-BA2D-36262B0F6044}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="940" windowWidth="19820" windowHeight="16980" activeTab="1" xr2:uid="{ECDB7163-6CBA-1844-B026-8197D854D89A}"/>
+    <workbookView xWindow="2540" yWindow="1020" windowWidth="19820" windowHeight="16980" activeTab="1" xr2:uid="{ECDB7163-6CBA-1844-B026-8197D854D89A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
   <connection id="1" xr16:uid="{9415BF77-C037-2345-896B-FAF71B77AB1B}" name="aparc.annot.DKTatlas" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/m206305/Documents/data/BrainBeat/data/aparc.annot.DKTatlas.txt" delimited="0">
+    <textPr sourceFile="/Users/m206305/Documents/data/BrainBeat/data/aparc.annot.DKTatlas.txt" delimited="0">
       <textFields count="6">
         <textField/>
         <textField position="3"/>
@@ -2728,10 +2728,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4F7138C-DF60-2440-AC0D-D41425418D54}">
-  <dimension ref="A1:M37"/>
+  <dimension ref="A1:R37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16:M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2744,7 +2744,7 @@
     <col min="9" max="9" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>143</v>
       </c>
@@ -2782,7 +2782,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2823,7 +2823,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2864,7 +2864,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2896,16 +2896,16 @@
         <v>1002</v>
       </c>
       <c r="K4">
-        <v>0.76</v>
+        <v>0.85</v>
       </c>
       <c r="L4">
-        <v>0.2</v>
+        <v>0.26</v>
       </c>
       <c r="M4">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2937,16 +2937,16 @@
         <v>3004</v>
       </c>
       <c r="K5">
-        <v>0.45</v>
+        <v>0.8</v>
       </c>
       <c r="L5">
-        <v>0.45</v>
+        <v>0.8</v>
       </c>
       <c r="M5">
-        <v>0.73</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2987,7 +2987,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3019,16 +3019,16 @@
         <v>2003</v>
       </c>
       <c r="K7">
-        <v>0.4</v>
+        <v>0.53</v>
       </c>
       <c r="L7">
-        <v>0.73</v>
+        <v>0.85</v>
       </c>
       <c r="M7">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+        <v>0.53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3060,16 +3060,16 @@
         <v>4001</v>
       </c>
       <c r="K8">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="L8">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="M8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3101,16 +3101,16 @@
         <v>2003</v>
       </c>
       <c r="K9">
-        <v>0.4</v>
+        <v>0.53</v>
       </c>
       <c r="L9">
-        <v>0.73</v>
+        <v>0.85</v>
       </c>
       <c r="M9">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+        <v>0.53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3142,16 +3142,16 @@
         <v>3004</v>
       </c>
       <c r="K10">
-        <v>0.45</v>
+        <v>0.8</v>
       </c>
       <c r="L10">
-        <v>0.45</v>
+        <v>0.8</v>
       </c>
       <c r="M10">
-        <v>0.73</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3183,16 +3183,16 @@
         <v>2004</v>
       </c>
       <c r="K11">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="L11">
-        <v>0.7</v>
+        <v>0.85</v>
       </c>
       <c r="M11">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3224,16 +3224,16 @@
         <v>1004</v>
       </c>
       <c r="K12">
-        <v>0.7</v>
+        <v>0.85</v>
       </c>
       <c r="L12">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="M12">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3262,19 +3262,19 @@
         <v>9</v>
       </c>
       <c r="J13">
-        <v>3005</v>
+        <v>2004</v>
       </c>
       <c r="K13">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="L13">
-        <v>0.6</v>
+        <v>0.85</v>
       </c>
       <c r="M13">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3306,16 +3306,16 @@
         <v>3004</v>
       </c>
       <c r="K14">
-        <v>0.45</v>
+        <v>0.8</v>
       </c>
       <c r="L14">
-        <v>0.45</v>
+        <v>0.8</v>
       </c>
       <c r="M14">
-        <v>0.73</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3347,16 +3347,16 @@
         <v>2002</v>
       </c>
       <c r="K15">
-        <v>0.2</v>
+        <v>0.26</v>
       </c>
       <c r="L15">
-        <v>0.76</v>
+        <v>0.85</v>
       </c>
       <c r="M15">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3385,16 +3385,28 @@
         <v>12</v>
       </c>
       <c r="J16">
+        <v>1001</v>
+      </c>
+      <c r="K16">
+        <v>0.5</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="O16">
         <v>1002</v>
       </c>
-      <c r="K16">
-        <v>0.76</v>
-      </c>
-      <c r="L16">
-        <v>0.2</v>
-      </c>
-      <c r="M16">
-        <v>0.2</v>
+      <c r="P16">
+        <v>0.85</v>
+      </c>
+      <c r="Q16">
+        <v>0.26</v>
+      </c>
+      <c r="R16">
+        <v>0.26</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
@@ -3429,13 +3441,13 @@
         <v>3004</v>
       </c>
       <c r="K17">
-        <v>0.65</v>
+        <v>0.8</v>
       </c>
       <c r="L17">
-        <v>0.65</v>
+        <v>0.8</v>
       </c>
       <c r="M17">
-        <v>0.77</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
@@ -3473,7 +3485,7 @@
         <v>0</v>
       </c>
       <c r="L18">
-        <v>0.8</v>
+        <v>0.5</v>
       </c>
       <c r="M18">
         <v>0</v>
@@ -3511,13 +3523,13 @@
         <v>1004</v>
       </c>
       <c r="K19">
-        <v>0.7</v>
+        <v>0.85</v>
       </c>
       <c r="L19">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="M19">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
@@ -3549,16 +3561,16 @@
         <v>16</v>
       </c>
       <c r="J20">
-        <v>3003</v>
+        <v>3002</v>
       </c>
       <c r="K20">
-        <v>0.3</v>
+        <v>0.26</v>
       </c>
       <c r="L20">
-        <v>0.3</v>
+        <v>0.26</v>
       </c>
       <c r="M20">
-        <v>0.75</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
@@ -3590,16 +3602,16 @@
         <v>17</v>
       </c>
       <c r="J21">
-        <v>3003</v>
+        <v>3002</v>
       </c>
       <c r="K21">
-        <v>0.3</v>
+        <v>0.26</v>
       </c>
       <c r="L21">
-        <v>0.3</v>
+        <v>0.26</v>
       </c>
       <c r="M21">
-        <v>0.75</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
@@ -3631,16 +3643,16 @@
         <v>18</v>
       </c>
       <c r="J22">
-        <v>3003</v>
+        <v>3002</v>
       </c>
       <c r="K22">
-        <v>0.3</v>
+        <v>0.26</v>
       </c>
       <c r="L22">
-        <v>0.3</v>
+        <v>0.26</v>
       </c>
       <c r="M22">
-        <v>0.75</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
@@ -3675,13 +3687,13 @@
         <v>2002</v>
       </c>
       <c r="K23">
-        <v>0.2</v>
+        <v>0.26</v>
       </c>
       <c r="L23">
-        <v>0.76</v>
+        <v>0.85</v>
       </c>
       <c r="M23">
-        <v>0.2</v>
+        <v>0.26</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
@@ -3716,13 +3728,13 @@
         <v>3004</v>
       </c>
       <c r="K24">
-        <v>0.45</v>
+        <v>0.8</v>
       </c>
       <c r="L24">
-        <v>0.45</v>
+        <v>0.8</v>
       </c>
       <c r="M24">
-        <v>0.73</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
@@ -3757,13 +3769,13 @@
         <v>1003</v>
       </c>
       <c r="K25">
-        <v>0.73</v>
+        <v>0.85</v>
       </c>
       <c r="L25">
-        <v>0.4</v>
+        <v>0.53</v>
       </c>
       <c r="M25">
-        <v>0.4</v>
+        <v>0.53</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
@@ -3798,13 +3810,13 @@
         <v>3004</v>
       </c>
       <c r="K26">
-        <v>0.45</v>
+        <v>0.8</v>
       </c>
       <c r="L26">
-        <v>0.45</v>
+        <v>0.8</v>
       </c>
       <c r="M26">
-        <v>0.73</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
@@ -3839,13 +3851,13 @@
         <v>1004</v>
       </c>
       <c r="K27">
-        <v>0.7</v>
+        <v>0.85</v>
       </c>
       <c r="L27">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="M27">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
@@ -3880,7 +3892,7 @@
         <v>1001</v>
       </c>
       <c r="K28">
-        <v>0.8</v>
+        <v>0.5</v>
       </c>
       <c r="L28">
         <v>0</v>
@@ -3921,13 +3933,13 @@
         <v>3004</v>
       </c>
       <c r="K29">
-        <v>0.45</v>
+        <v>0.8</v>
       </c>
       <c r="L29">
-        <v>0.45</v>
+        <v>0.8</v>
       </c>
       <c r="M29">
-        <v>0.73</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
@@ -3962,13 +3974,13 @@
         <v>1003</v>
       </c>
       <c r="K30">
-        <v>0.73</v>
+        <v>0.85</v>
       </c>
       <c r="L30">
-        <v>0.4</v>
+        <v>0.53</v>
       </c>
       <c r="M30">
-        <v>0.4</v>
+        <v>0.53</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
@@ -4003,13 +4015,13 @@
         <v>3004</v>
       </c>
       <c r="K31">
-        <v>0.45</v>
+        <v>0.8</v>
       </c>
       <c r="L31">
-        <v>0.45</v>
+        <v>0.8</v>
       </c>
       <c r="M31">
-        <v>0.73</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
@@ -4041,16 +4053,16 @@
         <v>28</v>
       </c>
       <c r="J32">
-        <v>3003</v>
+        <v>3002</v>
       </c>
       <c r="K32">
-        <v>0.3</v>
+        <v>0.26</v>
       </c>
       <c r="L32">
-        <v>0.3</v>
+        <v>0.26</v>
       </c>
       <c r="M32">
-        <v>0.75</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
@@ -4085,13 +4097,13 @@
         <v>3003</v>
       </c>
       <c r="K33">
-        <v>0.3</v>
+        <v>0.53</v>
       </c>
       <c r="L33">
-        <v>0.3</v>
+        <v>0.53</v>
       </c>
       <c r="M33">
-        <v>0.75</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
@@ -4167,13 +4179,13 @@
         <v>3004</v>
       </c>
       <c r="K35">
-        <v>0.65</v>
+        <v>0.8</v>
       </c>
       <c r="L35">
-        <v>0.65</v>
+        <v>0.8</v>
       </c>
       <c r="M35">
-        <v>0.77</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
@@ -4205,16 +4217,16 @@
         <v>30</v>
       </c>
       <c r="J36">
-        <v>3002</v>
+        <v>3001</v>
       </c>
       <c r="K36">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="L36">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="M36">
-        <v>0.78</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
@@ -4255,7 +4267,7 @@
         <v>0</v>
       </c>
       <c r="M37">
-        <v>0.8</v>
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>